<commit_message>
Made the dynamic selector click on the buttons
</commit_message>
<xml_diff>
--- a/followers.xlsx
+++ b/followers.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
+  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\The Rpa_Developer\RPA_PROJECTS\soundcloud\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="0"/>
 </x:workbook>
 </file>
 
@@ -19,88 +25,87 @@
     <x:t>Column1</x:t>
   </x:si>
   <x:si>
-    <x:t>Jennifer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Diselecta energy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BeisN Records</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rotimi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kovitch Officiel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>mr_empire</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DonJazzy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Positiva 860 AM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mr.LAWH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Radio620</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Numb Music</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C2o</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Willie F Da Room</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Valor Agregado</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MeredithComm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>revistaverdeuy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Anthony Rogers Show</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mackenzie Winger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kenzie Smith</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ruturaj Patil</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tasha Noguez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>wispolitics</x:t>
-  </x:si>
-  <x:si>
-    <x:t>chavcharm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LaCasaDeAutomatico</x:t>
+    <x:t xml:space="preserve"> LiamB </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Puff it </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Ayhan Uysal </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> ABKTRAUMA </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Deciffer </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> soo </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Lomax </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Roddy Ricch </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> TABradio </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Naija Lyrics </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Dj Tizo97 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> MethaPhorce Beats </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Swami Sounds </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Brandon From Addison </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Young Moé </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> William Birch </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Charlie Smith </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> User 294892344 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Kevin Cartwright </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Harrison Garner </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> ahmarimulkey2 </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Donnie Barney </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Emily Denton </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Kiing Prodigy </x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="1" x14ac:knownFonts="1">
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -116,30 +121,22 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -148,10 +145,19 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -434,139 +440,144 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:A25"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A9" sqref="A9 A9:A9"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="22.425781" style="1" bestFit="1" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:1">
-      <x:c r="A1" s="0" t="s">
+    <x:row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:1">
-      <x:c r="A2" s="0" t="s">
+    <x:row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:1">
-      <x:c r="A3" s="0" t="s">
+    <x:row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:1">
-      <x:c r="A4" s="0" t="s">
+    <x:row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:1">
-      <x:c r="A5" s="0" t="s">
+    <x:row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:1">
-      <x:c r="A6" s="0" t="s">
+    <x:row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:1">
-      <x:c r="A7" s="0" t="s">
+    <x:row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:1">
-      <x:c r="A8" s="0" t="s">
+    <x:row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="1" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:1">
-      <x:c r="A9" s="0" t="s">
+    <x:row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="1" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:1">
-      <x:c r="A10" s="0" t="s">
+    <x:row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="1" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:1">
-      <x:c r="A11" s="0" t="s">
+    <x:row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="1" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:1">
-      <x:c r="A12" s="0" t="s">
+    <x:row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="1" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:1">
-      <x:c r="A13" s="0" t="s">
+    <x:row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="1" t="s">
         <x:v>12</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:1">
-      <x:c r="A14" s="0" t="s">
+    <x:row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="1" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:1">
-      <x:c r="A15" s="0" t="s">
+    <x:row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="1" t="s">
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:1">
-      <x:c r="A16" s="0" t="s">
+    <x:row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A16" s="1" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:1">
-      <x:c r="A17" s="0" t="s">
+    <x:row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A17" s="1" t="s">
         <x:v>16</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:1">
-      <x:c r="A18" s="0" t="s">
+    <x:row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="1" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:1">
-      <x:c r="A19" s="0" t="s">
+    <x:row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A19" s="1" t="s">
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:1">
-      <x:c r="A20" s="0" t="s">
+    <x:row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A20" s="1" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:1">
-      <x:c r="A21" s="0" t="s">
+    <x:row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A21" s="1" t="s">
         <x:v>20</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:1">
-      <x:c r="A22" s="0" t="s">
+    <x:row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A22" s="1" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="23" spans="1:1">
-      <x:c r="A23" s="0" t="s">
+    <x:row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A23" s="1" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:1">
-      <x:c r="A24" s="0" t="s">
+    <x:row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A24" s="1" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="25" spans="1:1">
-      <x:c r="A25" s="0" t="s">
+    <x:row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A25" s="1" t="s">
         <x:v>24</x:v>
       </x:c>
     </x:row>

</xml_diff>